<commit_message>
moved things over to use new CRUD manager models
</commit_message>
<xml_diff>
--- a/hqbilling/static/hqbilling/files/mach-rate-example.xlsx
+++ b/hqbilling/static/hqbilling/files/mach-rate-example.xlsx
@@ -42,9 +42,6 @@
     <t>base_fee</t>
   </si>
   <si>
-    <t>surcharge</t>
-  </si>
-  <si>
     <t>mt_price</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>direction (I for Incoming O for Outgoing)</t>
+  </si>
+  <si>
+    <t>network_surcharge</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -451,16 +451,16 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>